<commit_message>
1. The program can use a subset of nmr data to solve problem 2. New xy dialog to choose what data gets used. 3. No longer needed to specify elements and number in molecule sheet 4. When no command line args program goes straigth to main screen. 5. This version is now official starting at 0.0.1 6. created pyinstaller spec file to make standalone windows and mac    versions of program
</commit_message>
<xml_diff>
--- a/exampleProblems/2-ethyl-1-indanone/ethyl_indanone.xlsx
+++ b/exampleProblems/2-ethyl-1-indanone/ethyl_indanone.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://durhamuniversity-my.sharepoint.com/personal/vsmw51_durham_ac_uk/Documents/projects/programming/2022/python/python/rdkit37/projects/simpleNMR/exampleProblems/2-ethyl-1-indanone/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="37" documentId="11_1B5B6F352AD0005635F3E51CCB4B55276CBFB855" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8A147112-185B-472A-9FAD-55E896AA3135}"/>
+  <xr:revisionPtr revIDLastSave="39" documentId="11_1B5B6F352AD0005635F3E51CCB4B55276CBFB855" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{27761461-E721-7249-A1C0-F4078E4E885E}"/>
   <bookViews>
-    <workbookView xWindow="4125" yWindow="1980" windowWidth="23880" windowHeight="13620" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4120" yWindow="1980" windowWidth="23880" windowHeight="13620" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="molecule" sheetId="9" r:id="rId1"/>
@@ -236,7 +236,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -406,6 +406,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -677,13 +681,13 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="B1" t="s">
         <v>62</v>
       </c>
@@ -691,7 +695,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -715,12 +719,12 @@
       <selection activeCell="C2" sqref="C2:C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="8" max="8" width="32.7109375" customWidth="1"/>
+    <col min="8" max="8" width="32.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -747,7 +751,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -776,7 +780,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -805,7 +809,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -834,7 +838,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -863,7 +867,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -892,7 +896,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -921,7 +925,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -950,7 +954,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -979,7 +983,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -1008,7 +1012,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9">
       <c r="A11" s="7">
         <v>10</v>
       </c>
@@ -1051,9 +1055,9 @@
       <selection sqref="A1:K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:13" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="24">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
         <v>57</v>
@@ -1086,7 +1090,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -1118,7 +1122,7 @@
       <c r="K2" s="6"/>
       <c r="M2" s="1"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -1150,7 +1154,7 @@
       <c r="K3" s="6"/>
       <c r="M3" s="1"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -1182,7 +1186,7 @@
       <c r="K4" s="6"/>
       <c r="M4" s="1"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -1214,7 +1218,7 @@
       <c r="K5" s="6"/>
       <c r="M5" s="1"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -1245,7 +1249,7 @@
       <c r="J6" s="1"/>
       <c r="K6" s="6"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -1277,7 +1281,7 @@
       <c r="K7" s="6"/>
       <c r="M7" s="1"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -1309,7 +1313,7 @@
       <c r="K8" s="6"/>
       <c r="M8" s="1"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -1341,7 +1345,7 @@
       <c r="K9" s="6"/>
       <c r="M9" s="1"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -1373,7 +1377,7 @@
       <c r="K10" s="6"/>
       <c r="M10" s="1"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13">
       <c r="A11" s="7">
         <v>10</v>
       </c>
@@ -1405,10 +1409,10 @@
       <c r="K11" s="9"/>
       <c r="M11" s="1"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13">
       <c r="M14" s="1"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13">
       <c r="M15" s="8"/>
     </row>
   </sheetData>
@@ -1423,9 +1427,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:22" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" ht="24">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
         <v>57</v>
@@ -1469,7 +1473,7 @@
       <c r="U1" s="3"/>
       <c r="V1" s="4"/>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -1502,7 +1506,7 @@
       <c r="U2" s="1"/>
       <c r="V2" s="6"/>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -1535,7 +1539,7 @@
       <c r="U3" s="1"/>
       <c r="V3" s="6"/>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -1568,7 +1572,7 @@
       <c r="U4" s="1"/>
       <c r="V4" s="6"/>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -1601,7 +1605,7 @@
       <c r="U5" s="1"/>
       <c r="V5" s="6"/>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -1634,7 +1638,7 @@
       <c r="U6" s="1"/>
       <c r="V6" s="6"/>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -1667,7 +1671,7 @@
       <c r="U7" s="1"/>
       <c r="V7" s="6"/>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -1700,7 +1704,7 @@
       <c r="U8" s="1"/>
       <c r="V8" s="6"/>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -1733,7 +1737,7 @@
       <c r="U9" s="1"/>
       <c r="V9" s="6"/>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -1766,7 +1770,7 @@
       <c r="U10" s="1"/>
       <c r="V10" s="6"/>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -1799,7 +1803,7 @@
       <c r="U11" s="1"/>
       <c r="V11" s="6"/>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22">
       <c r="A12" s="7">
         <v>11</v>
       </c>
@@ -1832,7 +1836,7 @@
       <c r="U12" s="1"/>
       <c r="V12" s="6"/>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22">
       <c r="A13" s="5"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -1847,7 +1851,7 @@
       <c r="U13" s="1"/>
       <c r="V13" s="6"/>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22">
       <c r="A14" s="5"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -1862,7 +1866,7 @@
       <c r="U14" s="1"/>
       <c r="V14" s="6"/>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22">
       <c r="A15" s="5"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1877,7 +1881,7 @@
       <c r="U15" s="1"/>
       <c r="V15" s="6"/>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22">
       <c r="A16" s="5"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1892,7 +1896,7 @@
       <c r="U16" s="1"/>
       <c r="V16" s="6"/>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:22">
       <c r="A17" s="7"/>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
@@ -1907,7 +1911,7 @@
       <c r="U17" s="8"/>
       <c r="V17" s="9"/>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:22">
       <c r="A18" s="5"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1931,7 +1935,7 @@
       <c r="U18" s="8"/>
       <c r="V18" s="9"/>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:22">
       <c r="A19" s="5"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1942,7 +1946,7 @@
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:22">
       <c r="A20" s="5"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1953,7 +1957,7 @@
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:22">
       <c r="A21" s="5"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1964,7 +1968,7 @@
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22">
       <c r="A22" s="5"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1975,7 +1979,7 @@
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:22">
       <c r="A23" s="5"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1986,7 +1990,7 @@
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:22">
       <c r="A24" s="5"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1997,7 +2001,7 @@
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:22">
       <c r="A25" s="5"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -2008,7 +2012,7 @@
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:22">
       <c r="A26" s="5"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -2019,7 +2023,7 @@
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:22">
       <c r="A27" s="5"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -2030,7 +2034,7 @@
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:22">
       <c r="A28" s="5"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -2041,7 +2045,7 @@
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:22">
       <c r="A29" s="5"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -2052,7 +2056,7 @@
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:22">
       <c r="A30" s="5"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -2063,7 +2067,7 @@
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:22">
       <c r="A31" s="5"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -2074,7 +2078,7 @@
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:22">
       <c r="A32" s="5"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -2085,7 +2089,7 @@
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9">
       <c r="A33" s="7"/>
       <c r="B33" s="8"/>
       <c r="C33" s="8"/>
@@ -2096,7 +2100,7 @@
       <c r="H33" s="8"/>
       <c r="I33" s="8"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9">
       <c r="A34" s="5"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -2107,7 +2111,7 @@
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9">
       <c r="A35" s="7"/>
       <c r="B35" s="8"/>
       <c r="C35" s="8"/>
@@ -2128,13 +2132,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:V45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:22" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" ht="24">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
         <v>57</v>
@@ -2178,27 +2182,27 @@
       <c r="U1" s="3"/>
       <c r="V1" s="4"/>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22">
       <c r="A2" s="5">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>2.6070000000000002</v>
+        <v>7.7389999999999999</v>
       </c>
       <c r="C2" s="1">
-        <v>209.09</v>
+        <v>134.55000000000001</v>
       </c>
       <c r="D2" s="1">
-        <v>3.1E-2</v>
+        <v>3.2000000000000001E-2</v>
       </c>
       <c r="E2" s="1">
-        <v>9.02</v>
+        <v>5.98</v>
       </c>
       <c r="F2" s="1">
-        <v>46.73</v>
+        <v>77.73</v>
       </c>
       <c r="G2" s="1">
-        <v>0.52</v>
+        <v>0.6</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>55</v>
@@ -2211,27 +2215,27 @@
       <c r="U2" s="1"/>
       <c r="V2" s="6"/>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22">
       <c r="A3" s="5">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1">
-        <v>2.6070000000000002</v>
+        <v>7.7389999999999999</v>
       </c>
       <c r="C3" s="1">
-        <v>24.42</v>
+        <v>153.74</v>
       </c>
       <c r="D3" s="1">
-        <v>4.2999999999999997E-2</v>
+        <v>1.6E-2</v>
       </c>
       <c r="E3" s="1">
-        <v>28.56</v>
+        <v>4.88</v>
       </c>
       <c r="F3" s="1">
-        <v>49.79</v>
+        <v>87.93</v>
       </c>
       <c r="G3" s="1">
-        <v>2.4500000000000002</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>55</v>
@@ -2244,27 +2248,27 @@
       <c r="U3" s="1"/>
       <c r="V3" s="6"/>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22">
       <c r="A4" s="5">
-        <v>35</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1">
-        <v>1.002</v>
+        <v>7.7380000000000004</v>
       </c>
       <c r="C4" s="1">
-        <v>24.69</v>
+        <v>208.96</v>
       </c>
       <c r="D4" s="1">
-        <v>0.13600000000000001</v>
+        <v>1.7000000000000001E-2</v>
       </c>
       <c r="E4" s="1">
-        <v>9.34</v>
+        <v>7.29</v>
       </c>
       <c r="F4" s="1">
-        <v>50.52</v>
+        <v>54.24</v>
       </c>
       <c r="G4" s="1">
-        <v>2.56</v>
+        <v>0.27</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>55</v>
@@ -2277,27 +2281,27 @@
       <c r="U4" s="1"/>
       <c r="V4" s="6"/>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22">
       <c r="A5" s="5">
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1">
-        <v>1.964</v>
+        <v>7.5670000000000002</v>
       </c>
       <c r="C5" s="1">
-        <v>11.63</v>
+        <v>123.79</v>
       </c>
       <c r="D5" s="1">
-        <v>7.0000000000000001E-3</v>
+        <v>3.1E-2</v>
       </c>
       <c r="E5" s="1">
-        <v>5.17</v>
+        <v>6.46</v>
       </c>
       <c r="F5" s="1">
-        <v>51.26</v>
+        <v>79.55</v>
       </c>
       <c r="G5" s="1">
-        <v>0.08</v>
+        <v>0.64</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>55</v>
@@ -2310,27 +2314,27 @@
       <c r="U5" s="1"/>
       <c r="V5" s="6"/>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22">
       <c r="A6" s="5">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="B6" s="1">
-        <v>1.532</v>
+        <v>7.5670000000000002</v>
       </c>
       <c r="C6" s="1">
-        <v>208.94</v>
+        <v>153.91999999999999</v>
       </c>
       <c r="D6" s="1">
-        <v>2.7E-2</v>
+        <v>0.03</v>
       </c>
       <c r="E6" s="1">
-        <v>7.69</v>
+        <v>6.36</v>
       </c>
       <c r="F6" s="1">
-        <v>53.43</v>
+        <v>84.84</v>
       </c>
       <c r="G6" s="1">
-        <v>0.45</v>
+        <v>0.64</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>55</v>
@@ -2343,27 +2347,27 @@
       <c r="U6" s="1"/>
       <c r="V6" s="6"/>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22">
       <c r="A7" s="5">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="B7" s="1">
-        <v>1.532</v>
+        <v>7.45</v>
       </c>
       <c r="C7" s="1">
-        <v>11.56</v>
+        <v>32.340000000000003</v>
       </c>
       <c r="D7" s="1">
-        <v>1.7000000000000001E-2</v>
+        <v>1.4E-2</v>
       </c>
       <c r="E7" s="1">
-        <v>5.29</v>
+        <v>8.94</v>
       </c>
       <c r="F7" s="1">
-        <v>53.47</v>
+        <v>82.91</v>
       </c>
       <c r="G7" s="1">
-        <v>0.19</v>
+        <v>0.41</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>55</v>
@@ -2376,27 +2380,27 @@
       <c r="U7" s="1"/>
       <c r="V7" s="6"/>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22">
       <c r="A8" s="5">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="B8" s="1">
-        <v>1.966</v>
+        <v>7.45</v>
       </c>
       <c r="C8" s="1">
-        <v>209.05</v>
+        <v>137.01</v>
       </c>
       <c r="D8" s="1">
-        <v>1.6E-2</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="E8" s="1">
-        <v>5.0199999999999996</v>
+        <v>4.97</v>
       </c>
       <c r="F8" s="1">
-        <v>53.74</v>
+        <v>87.04</v>
       </c>
       <c r="G8" s="1">
-        <v>0.17</v>
+        <v>0.26</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>55</v>
@@ -2409,27 +2413,27 @@
       <c r="U8" s="1"/>
       <c r="V8" s="6"/>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22">
       <c r="A9" s="5">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B9" s="1">
-        <v>7.7380000000000004</v>
+        <v>7.4489999999999998</v>
       </c>
       <c r="C9" s="1">
-        <v>208.96</v>
+        <v>127.26</v>
       </c>
       <c r="D9" s="1">
-        <v>1.7000000000000001E-2</v>
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="E9" s="1">
-        <v>7.29</v>
+        <v>4.2</v>
       </c>
       <c r="F9" s="1">
-        <v>54.24</v>
+        <v>69.680000000000007</v>
       </c>
       <c r="G9" s="1">
-        <v>0.27</v>
+        <v>0.22</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>55</v>
@@ -2442,27 +2446,27 @@
       <c r="U9" s="1"/>
       <c r="V9" s="6"/>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22">
       <c r="A10" s="5">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B10" s="1">
-        <v>3.31</v>
+        <v>7.4480000000000004</v>
       </c>
       <c r="C10" s="1">
-        <v>126.56</v>
+        <v>134.66</v>
       </c>
       <c r="D10" s="1">
-        <v>1.7999999999999999E-2</v>
+        <v>5.2999999999999999E-2</v>
       </c>
       <c r="E10" s="1">
-        <v>6.8</v>
+        <v>8.5399999999999991</v>
       </c>
       <c r="F10" s="1">
-        <v>54.81</v>
+        <v>80.34</v>
       </c>
       <c r="G10" s="1">
-        <v>0.26</v>
+        <v>1.44</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>55</v>
@@ -2470,32 +2474,32 @@
       <c r="I10" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="J10" s="1"/>
+      <c r="J10" s="13"/>
       <c r="K10" s="6"/>
       <c r="U10" s="1"/>
       <c r="V10" s="6"/>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22">
       <c r="A11" s="5">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="B11" s="1">
-        <v>2.6070000000000002</v>
+        <v>7.3470000000000004</v>
       </c>
       <c r="C11" s="1">
-        <v>11.65</v>
+        <v>137.09</v>
       </c>
       <c r="D11" s="1">
-        <v>1.7999999999999999E-2</v>
+        <v>0.03</v>
       </c>
       <c r="E11" s="1">
-        <v>22.63</v>
+        <v>5.7</v>
       </c>
       <c r="F11" s="1">
-        <v>55.19</v>
+        <v>83.6</v>
       </c>
       <c r="G11" s="1">
-        <v>0.91</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>55</v>
@@ -2508,27 +2512,27 @@
       <c r="U11" s="1"/>
       <c r="V11" s="6"/>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22">
       <c r="A12" s="5">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B12" s="1">
-        <v>3.3079999999999998</v>
+        <v>3.31</v>
       </c>
       <c r="C12" s="1">
-        <v>208.93</v>
+        <v>48.78</v>
       </c>
       <c r="D12" s="1">
-        <v>7.2999999999999995E-2</v>
+        <v>4.2999999999999997E-2</v>
       </c>
       <c r="E12" s="1">
-        <v>9.02</v>
+        <v>7.52</v>
       </c>
       <c r="F12" s="1">
-        <v>56.13</v>
+        <v>63.39</v>
       </c>
       <c r="G12" s="1">
-        <v>1.48</v>
+        <v>0.81</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>55</v>
@@ -2541,27 +2545,27 @@
       <c r="U12" s="1"/>
       <c r="V12" s="6"/>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22">
       <c r="A13" s="5">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B13" s="1">
-        <v>2.8130000000000002</v>
+        <v>3.31</v>
       </c>
       <c r="C13" s="1">
-        <v>126.59</v>
+        <v>126.56</v>
       </c>
       <c r="D13" s="1">
-        <v>3.0000000000000001E-3</v>
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="E13" s="1">
-        <v>8.42</v>
+        <v>6.8</v>
       </c>
       <c r="F13" s="1">
-        <v>56.84</v>
+        <v>54.81</v>
       </c>
       <c r="G13" s="1">
-        <v>7.0000000000000007E-2</v>
+        <v>0.26</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>55</v>
@@ -2574,27 +2578,27 @@
       <c r="U13" s="1"/>
       <c r="V13" s="6"/>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22">
       <c r="A14" s="5">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B14" s="1">
-        <v>2.8130000000000002</v>
+        <v>3.31</v>
       </c>
       <c r="C14" s="1">
-        <v>24.5</v>
+        <v>136.93</v>
       </c>
       <c r="D14" s="1">
-        <v>0.02</v>
+        <v>2.4E-2</v>
       </c>
       <c r="E14" s="1">
-        <v>8.8699999999999992</v>
+        <v>8.5500000000000007</v>
       </c>
       <c r="F14" s="1">
-        <v>57.02</v>
+        <v>86.42</v>
       </c>
       <c r="G14" s="1">
-        <v>0.41</v>
+        <v>0.7</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>55</v>
@@ -2607,27 +2611,27 @@
       <c r="U14" s="1"/>
       <c r="V14" s="6"/>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22">
       <c r="A15" s="5">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15" s="1">
-        <v>3.3090000000000002</v>
+        <v>3.31</v>
       </c>
       <c r="C15" s="1">
-        <v>24.45</v>
+        <v>153.87</v>
       </c>
       <c r="D15" s="1">
-        <v>1.9E-2</v>
+        <v>6.2E-2</v>
       </c>
       <c r="E15" s="1">
-        <v>5.83</v>
+        <v>6.77</v>
       </c>
       <c r="F15" s="1">
-        <v>58.75</v>
+        <v>89.84</v>
       </c>
       <c r="G15" s="1">
-        <v>0.26</v>
+        <v>1.5</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>55</v>
@@ -2640,27 +2644,27 @@
       <c r="U15" s="1"/>
       <c r="V15" s="6"/>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22">
       <c r="A16" s="5">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="B16" s="1">
-        <v>1.966</v>
+        <v>3.3090000000000002</v>
       </c>
       <c r="C16" s="1">
-        <v>48.79</v>
+        <v>24.45</v>
       </c>
       <c r="D16" s="1">
-        <v>1.6E-2</v>
+        <v>1.9E-2</v>
       </c>
       <c r="E16" s="1">
-        <v>6.01</v>
+        <v>5.83</v>
       </c>
       <c r="F16" s="1">
-        <v>62.6</v>
+        <v>58.75</v>
       </c>
       <c r="G16" s="1">
-        <v>0.24</v>
+        <v>0.26</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>55</v>
@@ -2673,27 +2677,27 @@
       <c r="U16" s="1"/>
       <c r="V16" s="6"/>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:22">
       <c r="A17" s="5">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B17" s="1">
-        <v>3.31</v>
+        <v>3.3079999999999998</v>
       </c>
       <c r="C17" s="1">
-        <v>48.78</v>
+        <v>208.93</v>
       </c>
       <c r="D17" s="1">
-        <v>4.2999999999999997E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="E17" s="1">
-        <v>7.52</v>
+        <v>9.02</v>
       </c>
       <c r="F17" s="1">
-        <v>63.39</v>
+        <v>56.13</v>
       </c>
       <c r="G17" s="1">
-        <v>0.81</v>
+        <v>1.48</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>55</v>
@@ -2706,27 +2710,27 @@
       <c r="U17" s="1"/>
       <c r="V17" s="6"/>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:22">
       <c r="A18" s="5">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="B18" s="1">
-        <v>1.0029999999999999</v>
+        <v>2.8140000000000001</v>
       </c>
       <c r="C18" s="1">
-        <v>48.77</v>
+        <v>153.86000000000001</v>
       </c>
       <c r="D18" s="1">
-        <v>0.28799999999999998</v>
+        <v>1.4E-2</v>
       </c>
       <c r="E18" s="1">
-        <v>5.13</v>
+        <v>5.72</v>
       </c>
       <c r="F18" s="1">
-        <v>66.13</v>
+        <v>90.27</v>
       </c>
       <c r="G18" s="1">
-        <v>3.9</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="H18" s="1" t="s">
         <v>55</v>
@@ -2739,7 +2743,7 @@
       <c r="U18" s="1"/>
       <c r="V18" s="6"/>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:22">
       <c r="A19" s="7">
         <v>18</v>
       </c>
@@ -2781,58 +2785,58 @@
       <c r="U19" s="11"/>
       <c r="V19" s="12"/>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:22">
       <c r="A20" s="5">
-        <v>8</v>
-      </c>
-      <c r="B20" s="13">
-        <v>7.4489999999999998</v>
-      </c>
-      <c r="C20" s="13">
-        <v>127.26</v>
-      </c>
-      <c r="D20" s="13">
-        <v>1.7999999999999999E-2</v>
-      </c>
-      <c r="E20" s="13">
-        <v>4.2</v>
-      </c>
-      <c r="F20" s="13">
-        <v>69.680000000000007</v>
-      </c>
-      <c r="G20" s="13">
-        <v>0.22</v>
-      </c>
-      <c r="H20" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="I20" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="J20" s="13"/>
+        <v>19</v>
+      </c>
+      <c r="B20" s="1">
+        <v>2.8130000000000002</v>
+      </c>
+      <c r="C20" s="1">
+        <v>24.5</v>
+      </c>
+      <c r="D20" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="E20" s="1">
+        <v>8.8699999999999992</v>
+      </c>
+      <c r="F20" s="1">
+        <v>57.02</v>
+      </c>
+      <c r="G20" s="1">
+        <v>0.41</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J20" s="1"/>
       <c r="K20" s="6"/>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:22">
       <c r="A21" s="5">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="B21" s="1">
-        <v>7.7389999999999999</v>
+        <v>2.8130000000000002</v>
       </c>
       <c r="C21" s="1">
-        <v>134.55000000000001</v>
+        <v>126.59</v>
       </c>
       <c r="D21" s="1">
-        <v>3.2000000000000001E-2</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="E21" s="1">
-        <v>5.98</v>
+        <v>8.42</v>
       </c>
       <c r="F21" s="1">
-        <v>77.73</v>
+        <v>56.84</v>
       </c>
       <c r="G21" s="1">
-        <v>0.6</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>55</v>
@@ -2843,27 +2847,27 @@
       <c r="J21" s="1"/>
       <c r="K21" s="6"/>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22">
       <c r="A22" s="5">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="B22" s="1">
-        <v>7.5670000000000002</v>
+        <v>2.8119999999999998</v>
       </c>
       <c r="C22" s="1">
-        <v>123.79</v>
+        <v>137.02000000000001</v>
       </c>
       <c r="D22" s="1">
-        <v>3.1E-2</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="E22" s="1">
-        <v>6.46</v>
+        <v>8.65</v>
       </c>
       <c r="F22" s="1">
-        <v>79.55</v>
+        <v>90.05</v>
       </c>
       <c r="G22" s="1">
-        <v>0.64</v>
+        <v>0.24</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>55</v>
@@ -2874,27 +2878,27 @@
       <c r="J22" s="1"/>
       <c r="K22" s="6"/>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:22">
       <c r="A23" s="5">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="B23" s="1">
-        <v>7.4480000000000004</v>
+        <v>2.8119999999999998</v>
       </c>
       <c r="C23" s="1">
-        <v>134.66</v>
+        <v>134.55000000000001</v>
       </c>
       <c r="D23" s="1">
-        <v>5.2999999999999999E-2</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="E23" s="1">
-        <v>8.5399999999999991</v>
+        <v>8.2200000000000006</v>
       </c>
       <c r="F23" s="1">
-        <v>80.34</v>
+        <v>81.86</v>
       </c>
       <c r="G23" s="1">
-        <v>1.44</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>55</v>
@@ -2905,27 +2909,27 @@
       <c r="J23" s="8"/>
       <c r="K23" s="9"/>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:22">
       <c r="A24" s="5">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B24" s="1">
-        <v>1.9670000000000001</v>
+        <v>2.6070000000000002</v>
       </c>
       <c r="C24" s="1">
-        <v>32.130000000000003</v>
+        <v>24.42</v>
       </c>
       <c r="D24" s="1">
-        <v>3.7999999999999999E-2</v>
+        <v>4.2999999999999997E-2</v>
       </c>
       <c r="E24" s="1">
-        <v>6.95</v>
+        <v>28.56</v>
       </c>
       <c r="F24" s="1">
-        <v>80.52</v>
+        <v>49.79</v>
       </c>
       <c r="G24" s="1">
-        <v>0.85</v>
+        <v>2.4500000000000002</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>55</v>
@@ -2936,27 +2940,27 @@
       <c r="J24" s="1"/>
       <c r="K24" s="6"/>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:22">
       <c r="A25" s="5">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B25" s="1">
-        <v>2.8119999999999998</v>
+        <v>2.6070000000000002</v>
       </c>
       <c r="C25" s="1">
-        <v>134.55000000000001</v>
+        <v>11.65</v>
       </c>
       <c r="D25" s="1">
-        <v>3.0000000000000001E-3</v>
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="E25" s="1">
-        <v>8.2200000000000006</v>
+        <v>22.63</v>
       </c>
       <c r="F25" s="1">
-        <v>81.86</v>
+        <v>55.19</v>
       </c>
       <c r="G25" s="1">
-        <v>7.0000000000000007E-2</v>
+        <v>0.91</v>
       </c>
       <c r="H25" s="1" t="s">
         <v>55</v>
@@ -2964,30 +2968,30 @@
       <c r="I25" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="J25" s="13"/>
+      <c r="J25" s="1"/>
       <c r="K25" s="6"/>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:22">
       <c r="A26" s="5">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="B26" s="1">
-        <v>7.45</v>
+        <v>2.6070000000000002</v>
       </c>
       <c r="C26" s="1">
-        <v>32.340000000000003</v>
+        <v>209.09</v>
       </c>
       <c r="D26" s="1">
-        <v>1.4E-2</v>
+        <v>3.1E-2</v>
       </c>
       <c r="E26" s="1">
-        <v>8.94</v>
+        <v>9.02</v>
       </c>
       <c r="F26" s="1">
-        <v>82.91</v>
+        <v>46.73</v>
       </c>
       <c r="G26" s="1">
-        <v>0.41</v>
+        <v>0.52</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>55</v>
@@ -2998,7 +3002,7 @@
       <c r="J26" s="1"/>
       <c r="K26" s="6"/>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:22">
       <c r="A27" s="5">
         <v>26</v>
       </c>
@@ -3029,27 +3033,27 @@
       <c r="J27" s="1"/>
       <c r="K27" s="6"/>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:22">
       <c r="A28" s="5">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="B28" s="1">
-        <v>7.3470000000000004</v>
+        <v>2.6059999999999999</v>
       </c>
       <c r="C28" s="1">
-        <v>137.09</v>
+        <v>153.76</v>
       </c>
       <c r="D28" s="1">
-        <v>0.03</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="E28" s="1">
-        <v>5.7</v>
+        <v>23.21</v>
       </c>
       <c r="F28" s="1">
-        <v>83.6</v>
+        <v>89.58</v>
       </c>
       <c r="G28" s="1">
-        <v>0.56999999999999995</v>
+        <v>2.09</v>
       </c>
       <c r="H28" s="1" t="s">
         <v>55</v>
@@ -3060,27 +3064,27 @@
       <c r="J28" s="1"/>
       <c r="K28" s="6"/>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:22">
       <c r="A29" s="5">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="B29" s="1">
-        <v>7.5670000000000002</v>
+        <v>1.9670000000000001</v>
       </c>
       <c r="C29" s="1">
-        <v>153.91999999999999</v>
+        <v>32.130000000000003</v>
       </c>
       <c r="D29" s="1">
-        <v>0.03</v>
+        <v>3.7999999999999999E-2</v>
       </c>
       <c r="E29" s="1">
-        <v>6.36</v>
+        <v>6.95</v>
       </c>
       <c r="F29" s="1">
-        <v>84.84</v>
+        <v>80.52</v>
       </c>
       <c r="G29" s="1">
-        <v>0.64</v>
+        <v>0.85</v>
       </c>
       <c r="H29" s="1" t="s">
         <v>55</v>
@@ -3091,27 +3095,27 @@
       <c r="J29" s="1"/>
       <c r="K29" s="6"/>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:22">
       <c r="A30" s="5">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="B30" s="1">
-        <v>3.31</v>
+        <v>1.966</v>
       </c>
       <c r="C30" s="1">
-        <v>136.93</v>
+        <v>48.79</v>
       </c>
       <c r="D30" s="1">
-        <v>2.4E-2</v>
+        <v>1.6E-2</v>
       </c>
       <c r="E30" s="1">
-        <v>8.5500000000000007</v>
+        <v>6.01</v>
       </c>
       <c r="F30" s="1">
-        <v>86.42</v>
+        <v>62.6</v>
       </c>
       <c r="G30" s="1">
-        <v>0.7</v>
+        <v>0.24</v>
       </c>
       <c r="H30" s="1" t="s">
         <v>55</v>
@@ -3119,30 +3123,30 @@
       <c r="I30" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="J30" s="13"/>
+      <c r="J30" s="1"/>
       <c r="K30" s="6"/>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:22">
       <c r="A31" s="5">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="B31" s="1">
-        <v>7.45</v>
+        <v>1.966</v>
       </c>
       <c r="C31" s="1">
-        <v>137.01</v>
+        <v>209.05</v>
       </c>
       <c r="D31" s="1">
-        <v>1.4999999999999999E-2</v>
+        <v>1.6E-2</v>
       </c>
       <c r="E31" s="1">
-        <v>4.97</v>
+        <v>5.0199999999999996</v>
       </c>
       <c r="F31" s="1">
-        <v>87.04</v>
+        <v>53.74</v>
       </c>
       <c r="G31" s="1">
-        <v>0.26</v>
+        <v>0.17</v>
       </c>
       <c r="H31" s="1" t="s">
         <v>55</v>
@@ -3153,27 +3157,27 @@
       <c r="J31" s="1"/>
       <c r="K31" s="6"/>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:22">
       <c r="A32" s="5">
-        <v>2</v>
+        <v>31</v>
       </c>
       <c r="B32" s="1">
-        <v>7.7389999999999999</v>
+        <v>1.964</v>
       </c>
       <c r="C32" s="1">
-        <v>153.74</v>
+        <v>11.63</v>
       </c>
       <c r="D32" s="1">
-        <v>1.6E-2</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="E32" s="1">
-        <v>4.88</v>
+        <v>5.17</v>
       </c>
       <c r="F32" s="1">
-        <v>87.93</v>
+        <v>51.26</v>
       </c>
       <c r="G32" s="1">
-        <v>0.28000000000000003</v>
+        <v>0.08</v>
       </c>
       <c r="H32" s="1" t="s">
         <v>55</v>
@@ -3184,27 +3188,27 @@
       <c r="J32" s="1"/>
       <c r="K32" s="6"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11">
       <c r="A33" s="5">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B33" s="1">
-        <v>2.6059999999999999</v>
+        <v>1.532</v>
       </c>
       <c r="C33" s="1">
-        <v>153.76</v>
+        <v>208.94</v>
       </c>
       <c r="D33" s="1">
-        <v>2.5000000000000001E-2</v>
+        <v>2.7E-2</v>
       </c>
       <c r="E33" s="1">
-        <v>23.21</v>
+        <v>7.69</v>
       </c>
       <c r="F33" s="1">
-        <v>89.58</v>
+        <v>53.43</v>
       </c>
       <c r="G33" s="1">
-        <v>2.09</v>
+        <v>0.45</v>
       </c>
       <c r="H33" s="1" t="s">
         <v>55</v>
@@ -3215,27 +3219,27 @@
       <c r="J33" s="1"/>
       <c r="K33" s="6"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11">
       <c r="A34" s="5">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="B34" s="1">
-        <v>3.31</v>
+        <v>1.532</v>
       </c>
       <c r="C34" s="1">
-        <v>153.87</v>
+        <v>11.56</v>
       </c>
       <c r="D34" s="1">
-        <v>6.2E-2</v>
+        <v>1.7000000000000001E-2</v>
       </c>
       <c r="E34" s="1">
-        <v>6.77</v>
+        <v>5.29</v>
       </c>
       <c r="F34" s="1">
-        <v>89.84</v>
+        <v>53.47</v>
       </c>
       <c r="G34" s="1">
-        <v>1.5</v>
+        <v>0.19</v>
       </c>
       <c r="H34" s="1" t="s">
         <v>55</v>
@@ -3246,27 +3250,27 @@
       <c r="J34" s="1"/>
       <c r="K34" s="6"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11">
       <c r="A35" s="5">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="B35" s="1">
-        <v>2.8119999999999998</v>
+        <v>1.0029999999999999</v>
       </c>
       <c r="C35" s="1">
-        <v>137.02000000000001</v>
+        <v>48.77</v>
       </c>
       <c r="D35" s="1">
-        <v>8.0000000000000002E-3</v>
+        <v>0.28799999999999998</v>
       </c>
       <c r="E35" s="1">
-        <v>8.65</v>
+        <v>5.13</v>
       </c>
       <c r="F35" s="1">
-        <v>90.05</v>
+        <v>66.13</v>
       </c>
       <c r="G35" s="1">
-        <v>0.24</v>
+        <v>3.9</v>
       </c>
       <c r="H35" s="1" t="s">
         <v>55</v>
@@ -3277,27 +3281,27 @@
       <c r="J35" s="1"/>
       <c r="K35" s="6"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11">
       <c r="A36" s="5">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="B36" s="1">
-        <v>2.8140000000000001</v>
+        <v>1.002</v>
       </c>
       <c r="C36" s="1">
-        <v>153.86000000000001</v>
+        <v>24.69</v>
       </c>
       <c r="D36" s="1">
-        <v>1.4E-2</v>
+        <v>0.13600000000000001</v>
       </c>
       <c r="E36" s="1">
-        <v>5.72</v>
+        <v>9.34</v>
       </c>
       <c r="F36" s="1">
-        <v>90.27</v>
+        <v>50.52</v>
       </c>
       <c r="G36" s="1">
-        <v>0.28000000000000003</v>
+        <v>2.56</v>
       </c>
       <c r="H36" s="1" t="s">
         <v>55</v>
@@ -3308,7 +3312,7 @@
       <c r="J36" s="1"/>
       <c r="K36" s="6"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11">
       <c r="A37" s="5"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -3321,7 +3325,7 @@
       <c r="J37" s="1"/>
       <c r="K37" s="6"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11">
       <c r="A38" s="5"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -3334,7 +3338,7 @@
       <c r="J38" s="1"/>
       <c r="K38" s="6"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11">
       <c r="A39" s="5"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -3347,7 +3351,7 @@
       <c r="J39" s="1"/>
       <c r="K39" s="6"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11">
       <c r="A40" s="5"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -3360,7 +3364,7 @@
       <c r="J40" s="1"/>
       <c r="K40" s="6"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11">
       <c r="A41" s="5"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -3373,7 +3377,7 @@
       <c r="J41" s="1"/>
       <c r="K41" s="6"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11">
       <c r="A42" s="5"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -3386,7 +3390,7 @@
       <c r="J42" s="1"/>
       <c r="K42" s="6"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11">
       <c r="A43" s="5"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -3399,7 +3403,7 @@
       <c r="J43" s="1"/>
       <c r="K43" s="6"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11">
       <c r="A44" s="5"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -3412,7 +3416,7 @@
       <c r="J44" s="1"/>
       <c r="K44" s="6"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11">
       <c r="A45" s="7"/>
       <c r="B45" s="8"/>
       <c r="C45" s="8"/>
@@ -3426,8 +3430,8 @@
       <c r="K45" s="9"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K45">
-    <sortCondition ref="F2:F45"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K46">
+    <sortCondition ref="A2:A46"/>
   </sortState>
   <mergeCells count="1">
     <mergeCell ref="L19:V19"/>
@@ -3445,9 +3449,9 @@
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="24">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
         <v>47</v>
@@ -3474,7 +3478,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -3499,7 +3503,7 @@
       <c r="H2" s="1"/>
       <c r="I2" s="6"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -3524,7 +3528,7 @@
       <c r="H3" s="1"/>
       <c r="I3" s="6"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -3549,7 +3553,7 @@
       <c r="H4" s="1"/>
       <c r="I4" s="6"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -3574,7 +3578,7 @@
       <c r="H5" s="1"/>
       <c r="I5" s="6"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -3599,7 +3603,7 @@
       <c r="H6" s="1"/>
       <c r="I6" s="6"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -3624,7 +3628,7 @@
       <c r="H7" s="1"/>
       <c r="I7" s="6"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -3649,7 +3653,7 @@
       <c r="H8" s="1"/>
       <c r="I8" s="6"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -3674,7 +3678,7 @@
       <c r="H9" s="1"/>
       <c r="I9" s="6"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -3699,7 +3703,7 @@
       <c r="H10" s="1"/>
       <c r="I10" s="6"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -3724,7 +3728,7 @@
       <c r="H11" s="1"/>
       <c r="I11" s="6"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9">
       <c r="A12" s="7">
         <v>11</v>
       </c>
@@ -3749,15 +3753,15 @@
       <c r="H12" s="1"/>
       <c r="I12" s="6"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9">
       <c r="H13" s="1"/>
       <c r="I13" s="6"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9">
       <c r="H14" s="1"/>
       <c r="I14" s="6"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9">
       <c r="H15" s="8"/>
       <c r="I15" s="9"/>
     </row>
@@ -3775,9 +3779,9 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="24">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
         <v>47</v>
@@ -3804,7 +3808,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -3829,7 +3833,7 @@
       <c r="H2" s="1"/>
       <c r="I2" s="6"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -3854,7 +3858,7 @@
       <c r="H3" s="1"/>
       <c r="I3" s="6"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -3879,7 +3883,7 @@
       <c r="H4" s="1"/>
       <c r="I4" s="6"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -3904,7 +3908,7 @@
       <c r="H5" s="1"/>
       <c r="I5" s="6"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -3929,7 +3933,7 @@
       <c r="H6" s="1"/>
       <c r="I6" s="6"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -3954,7 +3958,7 @@
       <c r="H7" s="1"/>
       <c r="I7" s="6"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -3979,7 +3983,7 @@
       <c r="H8" s="1"/>
       <c r="I8" s="6"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -4004,7 +4008,7 @@
       <c r="H9" s="1"/>
       <c r="I9" s="6"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -4029,7 +4033,7 @@
       <c r="H10" s="1"/>
       <c r="I10" s="6"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9">
       <c r="A11" s="7">
         <v>10</v>
       </c>
@@ -4054,10 +4058,10 @@
       <c r="H11" s="8"/>
       <c r="I11" s="9"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9">
       <c r="B12" s="8"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9">
       <c r="A14" s="2"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -4068,7 +4072,7 @@
       <c r="H14" s="3"/>
       <c r="I14" s="4"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9">
       <c r="A15" s="5"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -4079,7 +4083,7 @@
       <c r="H15" s="1"/>
       <c r="I15" s="6"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9">
       <c r="A16" s="5"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -4090,7 +4094,7 @@
       <c r="H16" s="1"/>
       <c r="I16" s="6"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9">
       <c r="A17" s="5"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -4101,7 +4105,7 @@
       <c r="H17" s="1"/>
       <c r="I17" s="6"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9">
       <c r="A18" s="5"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -4112,7 +4116,7 @@
       <c r="H18" s="1"/>
       <c r="I18" s="6"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9">
       <c r="A19" s="5"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -4123,7 +4127,7 @@
       <c r="H19" s="1"/>
       <c r="I19" s="6"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9">
       <c r="A20" s="5"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -4134,7 +4138,7 @@
       <c r="H20" s="1"/>
       <c r="I20" s="6"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9">
       <c r="A21" s="5"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -4145,7 +4149,7 @@
       <c r="H21" s="1"/>
       <c r="I21" s="6"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9">
       <c r="A22" s="5"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -4156,7 +4160,7 @@
       <c r="H22" s="1"/>
       <c r="I22" s="6"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9">
       <c r="A23" s="5"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -4167,7 +4171,7 @@
       <c r="H23" s="1"/>
       <c r="I23" s="6"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9">
       <c r="A24" s="5"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -4178,7 +4182,7 @@
       <c r="H24" s="1"/>
       <c r="I24" s="6"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9">
       <c r="A25" s="7"/>
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
@@ -4202,9 +4206,9 @@
       <selection sqref="A1:K3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="24">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
         <v>57</v>
@@ -4237,7 +4241,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -4268,7 +4272,7 @@
       <c r="J2" s="1"/>
       <c r="K2" s="6"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11">
       <c r="A3" s="7">
         <v>2</v>
       </c>
@@ -4306,6 +4310,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100155B07917A39914F9664B9093559A33D" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="fbeff89c08116489e82681c46e7ae15d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="f6191221-55a2-427d-afce-6bfcc029a585" xmlns:ns4="b60d6f15-5eb1-4c0b-bb71-d899d3bf026f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a905948312a67a3512ded1d64743b24d" ns3:_="" ns4:_="">
     <xsd:import namespace="f6191221-55a2-427d-afce-6bfcc029a585"/>
@@ -4522,22 +4541,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44668820-0664-4E62-A660-376AF03334EF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="b60d6f15-5eb1-4c0b-bb71-d899d3bf026f"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="f6191221-55a2-427d-afce-6bfcc029a585"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9421959D-9476-4FEC-BDFE-1367083D3EBE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CCEF473A-5319-4ED2-888F-44217AC86176}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4554,29 +4583,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9421959D-9476-4FEC-BDFE-1367083D3EBE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44668820-0664-4E62-A660-376AF03334EF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="f6191221-55a2-427d-afce-6bfcc029a585"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="b60d6f15-5eb1-4c0b-bb71-d899d3bf026f"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added a html page to show results which is access by CTrL-S
</commit_message>
<xml_diff>
--- a/exampleProblems/2-ethyl-1-indanone/ethyl_indanone.xlsx
+++ b/exampleProblems/2-ethyl-1-indanone/ethyl_indanone.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://durhamuniversity-my.sharepoint.com/personal/vsmw51_durham_ac_uk/Documents/projects/programming/2022/python/python/rdkit37/projects/simpleNMR/exampleProblems/2-ethyl-1-indanone/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="39" documentId="11_1B5B6F352AD0005635F3E51CCB4B55276CBFB855" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{27761461-E721-7249-A1C0-F4078E4E885E}"/>
+  <xr:revisionPtr revIDLastSave="45" documentId="11_1B5B6F352AD0005635F3E51CCB4B55276CBFB855" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CF9CD6E3-4261-4B4C-BDB4-C7BB509F55BF}"/>
   <bookViews>
-    <workbookView xWindow="4120" yWindow="1980" windowWidth="23880" windowHeight="13620" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8400" yWindow="0" windowWidth="16845" windowHeight="13875" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="molecule" sheetId="9" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="64">
   <si>
     <t>Name</t>
   </si>
@@ -218,12 +218,6 @@
   </si>
   <si>
     <t>Volume</t>
-  </si>
-  <si>
-    <t>molecule</t>
-  </si>
-  <si>
-    <t>C11H12O</t>
   </si>
   <si>
     <t>smiles</t>
@@ -236,7 +230,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -379,6 +373,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -387,9 +384,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -406,10 +400,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -675,35 +665,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>62</v>
       </c>
-      <c r="C1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>63</v>
-      </c>
-      <c r="C2" t="s">
-        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -719,12 +702,12 @@
       <selection activeCell="C2" sqref="C2:C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="8" max="8" width="32.6640625" customWidth="1"/>
+    <col min="8" max="8" width="32.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -751,7 +734,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -780,7 +763,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -809,7 +792,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -838,7 +821,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -867,7 +850,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -896,7 +879,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -925,7 +908,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -954,7 +937,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -983,7 +966,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -1012,7 +995,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>10</v>
       </c>
@@ -1055,9 +1038,9 @@
       <selection sqref="A1:K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:13" ht="24">
+    <row r="1" spans="1:13" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
         <v>57</v>
@@ -1090,7 +1073,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -1122,7 +1105,7 @@
       <c r="K2" s="6"/>
       <c r="M2" s="1"/>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -1154,7 +1137,7 @@
       <c r="K3" s="6"/>
       <c r="M3" s="1"/>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -1186,7 +1169,7 @@
       <c r="K4" s="6"/>
       <c r="M4" s="1"/>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -1218,7 +1201,7 @@
       <c r="K5" s="6"/>
       <c r="M5" s="1"/>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -1249,7 +1232,7 @@
       <c r="J6" s="1"/>
       <c r="K6" s="6"/>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -1281,7 +1264,7 @@
       <c r="K7" s="6"/>
       <c r="M7" s="1"/>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -1313,7 +1296,7 @@
       <c r="K8" s="6"/>
       <c r="M8" s="1"/>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -1345,7 +1328,7 @@
       <c r="K9" s="6"/>
       <c r="M9" s="1"/>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -1377,7 +1360,7 @@
       <c r="K10" s="6"/>
       <c r="M10" s="1"/>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>10</v>
       </c>
@@ -1409,10 +1392,10 @@
       <c r="K11" s="9"/>
       <c r="M11" s="1"/>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M14" s="1"/>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M15" s="8"/>
     </row>
   </sheetData>
@@ -1427,9 +1410,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:22" ht="24">
+    <row r="1" spans="1:22" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
         <v>57</v>
@@ -1473,7 +1456,7 @@
       <c r="U1" s="3"/>
       <c r="V1" s="4"/>
     </row>
-    <row r="2" spans="1:22">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -1506,7 +1489,7 @@
       <c r="U2" s="1"/>
       <c r="V2" s="6"/>
     </row>
-    <row r="3" spans="1:22">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -1539,7 +1522,7 @@
       <c r="U3" s="1"/>
       <c r="V3" s="6"/>
     </row>
-    <row r="4" spans="1:22">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -1572,7 +1555,7 @@
       <c r="U4" s="1"/>
       <c r="V4" s="6"/>
     </row>
-    <row r="5" spans="1:22">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -1605,7 +1588,7 @@
       <c r="U5" s="1"/>
       <c r="V5" s="6"/>
     </row>
-    <row r="6" spans="1:22">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -1638,7 +1621,7 @@
       <c r="U6" s="1"/>
       <c r="V6" s="6"/>
     </row>
-    <row r="7" spans="1:22">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -1671,7 +1654,7 @@
       <c r="U7" s="1"/>
       <c r="V7" s="6"/>
     </row>
-    <row r="8" spans="1:22">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -1704,7 +1687,7 @@
       <c r="U8" s="1"/>
       <c r="V8" s="6"/>
     </row>
-    <row r="9" spans="1:22">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -1737,7 +1720,7 @@
       <c r="U9" s="1"/>
       <c r="V9" s="6"/>
     </row>
-    <row r="10" spans="1:22">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -1770,7 +1753,7 @@
       <c r="U10" s="1"/>
       <c r="V10" s="6"/>
     </row>
-    <row r="11" spans="1:22">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -1803,7 +1786,7 @@
       <c r="U11" s="1"/>
       <c r="V11" s="6"/>
     </row>
-    <row r="12" spans="1:22">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
         <v>11</v>
       </c>
@@ -1836,7 +1819,7 @@
       <c r="U12" s="1"/>
       <c r="V12" s="6"/>
     </row>
-    <row r="13" spans="1:22">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -1851,7 +1834,7 @@
       <c r="U13" s="1"/>
       <c r="V13" s="6"/>
     </row>
-    <row r="14" spans="1:22">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -1866,7 +1849,7 @@
       <c r="U14" s="1"/>
       <c r="V14" s="6"/>
     </row>
-    <row r="15" spans="1:22">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1881,7 +1864,7 @@
       <c r="U15" s="1"/>
       <c r="V15" s="6"/>
     </row>
-    <row r="16" spans="1:22">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1896,7 +1879,7 @@
       <c r="U16" s="1"/>
       <c r="V16" s="6"/>
     </row>
-    <row r="17" spans="1:22">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
@@ -1911,7 +1894,7 @@
       <c r="U17" s="8"/>
       <c r="V17" s="9"/>
     </row>
-    <row r="18" spans="1:22">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1935,7 +1918,7 @@
       <c r="U18" s="8"/>
       <c r="V18" s="9"/>
     </row>
-    <row r="19" spans="1:22">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1946,7 +1929,7 @@
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="1:22">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1957,7 +1940,7 @@
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="1:22">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1968,7 +1951,7 @@
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:22">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1979,7 +1962,7 @@
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:22">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1990,7 +1973,7 @@
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
     </row>
-    <row r="24" spans="1:22">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -2001,7 +1984,7 @@
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
     </row>
-    <row r="25" spans="1:22">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -2012,7 +1995,7 @@
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
     </row>
-    <row r="26" spans="1:22">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -2023,7 +2006,7 @@
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
     </row>
-    <row r="27" spans="1:22">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -2034,7 +2017,7 @@
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
     </row>
-    <row r="28" spans="1:22">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -2045,7 +2028,7 @@
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
     </row>
-    <row r="29" spans="1:22">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A29" s="5"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -2056,7 +2039,7 @@
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
     </row>
-    <row r="30" spans="1:22">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A30" s="5"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -2067,7 +2050,7 @@
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
     </row>
-    <row r="31" spans="1:22">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -2078,7 +2061,7 @@
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
     </row>
-    <row r="32" spans="1:22">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A32" s="5"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -2089,7 +2072,7 @@
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="7"/>
       <c r="B33" s="8"/>
       <c r="C33" s="8"/>
@@ -2100,7 +2083,7 @@
       <c r="H33" s="8"/>
       <c r="I33" s="8"/>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="5"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -2111,7 +2094,7 @@
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="7"/>
       <c r="B35" s="8"/>
       <c r="C35" s="8"/>
@@ -2133,12 +2116,12 @@
   <dimension ref="A1:V45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="B2" sqref="A1:K36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:22" ht="24">
+    <row r="1" spans="1:22" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
         <v>57</v>
@@ -2182,7 +2165,7 @@
       <c r="U1" s="3"/>
       <c r="V1" s="4"/>
     </row>
-    <row r="2" spans="1:22">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -2215,7 +2198,7 @@
       <c r="U2" s="1"/>
       <c r="V2" s="6"/>
     </row>
-    <row r="3" spans="1:22">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -2248,7 +2231,7 @@
       <c r="U3" s="1"/>
       <c r="V3" s="6"/>
     </row>
-    <row r="4" spans="1:22">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -2281,7 +2264,7 @@
       <c r="U4" s="1"/>
       <c r="V4" s="6"/>
     </row>
-    <row r="5" spans="1:22">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -2314,7 +2297,7 @@
       <c r="U5" s="1"/>
       <c r="V5" s="6"/>
     </row>
-    <row r="6" spans="1:22">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -2347,7 +2330,7 @@
       <c r="U6" s="1"/>
       <c r="V6" s="6"/>
     </row>
-    <row r="7" spans="1:22">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -2380,7 +2363,7 @@
       <c r="U7" s="1"/>
       <c r="V7" s="6"/>
     </row>
-    <row r="8" spans="1:22">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -2413,7 +2396,7 @@
       <c r="U8" s="1"/>
       <c r="V8" s="6"/>
     </row>
-    <row r="9" spans="1:22">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -2446,7 +2429,7 @@
       <c r="U9" s="1"/>
       <c r="V9" s="6"/>
     </row>
-    <row r="10" spans="1:22">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -2474,12 +2457,12 @@
       <c r="I10" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="J10" s="13"/>
+      <c r="J10" s="10"/>
       <c r="K10" s="6"/>
       <c r="U10" s="1"/>
       <c r="V10" s="6"/>
     </row>
-    <row r="11" spans="1:22">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -2512,7 +2495,7 @@
       <c r="U11" s="1"/>
       <c r="V11" s="6"/>
     </row>
-    <row r="12" spans="1:22">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>11</v>
       </c>
@@ -2545,7 +2528,7 @@
       <c r="U12" s="1"/>
       <c r="V12" s="6"/>
     </row>
-    <row r="13" spans="1:22">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -2578,7 +2561,7 @@
       <c r="U13" s="1"/>
       <c r="V13" s="6"/>
     </row>
-    <row r="14" spans="1:22">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -2611,7 +2594,7 @@
       <c r="U14" s="1"/>
       <c r="V14" s="6"/>
     </row>
-    <row r="15" spans="1:22">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -2644,7 +2627,7 @@
       <c r="U15" s="1"/>
       <c r="V15" s="6"/>
     </row>
-    <row r="16" spans="1:22">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>15</v>
       </c>
@@ -2677,7 +2660,7 @@
       <c r="U16" s="1"/>
       <c r="V16" s="6"/>
     </row>
-    <row r="17" spans="1:22">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -2710,7 +2693,7 @@
       <c r="U17" s="1"/>
       <c r="V17" s="6"/>
     </row>
-    <row r="18" spans="1:22">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>17</v>
       </c>
@@ -2743,7 +2726,7 @@
       <c r="U18" s="1"/>
       <c r="V18" s="6"/>
     </row>
-    <row r="19" spans="1:22">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" s="7">
         <v>18</v>
       </c>
@@ -2773,19 +2756,19 @@
       </c>
       <c r="J19" s="8"/>
       <c r="K19" s="9"/>
-      <c r="L19" s="10"/>
-      <c r="M19" s="11"/>
-      <c r="N19" s="11"/>
-      <c r="O19" s="11"/>
-      <c r="P19" s="11"/>
-      <c r="Q19" s="11"/>
-      <c r="R19" s="11"/>
-      <c r="S19" s="11"/>
-      <c r="T19" s="11"/>
-      <c r="U19" s="11"/>
-      <c r="V19" s="12"/>
-    </row>
-    <row r="20" spans="1:22">
+      <c r="L19" s="11"/>
+      <c r="M19" s="12"/>
+      <c r="N19" s="12"/>
+      <c r="O19" s="12"/>
+      <c r="P19" s="12"/>
+      <c r="Q19" s="12"/>
+      <c r="R19" s="12"/>
+      <c r="S19" s="12"/>
+      <c r="T19" s="12"/>
+      <c r="U19" s="12"/>
+      <c r="V19" s="13"/>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>19</v>
       </c>
@@ -2816,7 +2799,7 @@
       <c r="J20" s="1"/>
       <c r="K20" s="6"/>
     </row>
-    <row r="21" spans="1:22">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>20</v>
       </c>
@@ -2847,7 +2830,7 @@
       <c r="J21" s="1"/>
       <c r="K21" s="6"/>
     </row>
-    <row r="22" spans="1:22">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>21</v>
       </c>
@@ -2878,7 +2861,7 @@
       <c r="J22" s="1"/>
       <c r="K22" s="6"/>
     </row>
-    <row r="23" spans="1:22">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>22</v>
       </c>
@@ -2909,7 +2892,7 @@
       <c r="J23" s="8"/>
       <c r="K23" s="9"/>
     </row>
-    <row r="24" spans="1:22">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>23</v>
       </c>
@@ -2940,7 +2923,7 @@
       <c r="J24" s="1"/>
       <c r="K24" s="6"/>
     </row>
-    <row r="25" spans="1:22">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>24</v>
       </c>
@@ -2971,7 +2954,7 @@
       <c r="J25" s="1"/>
       <c r="K25" s="6"/>
     </row>
-    <row r="26" spans="1:22">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>25</v>
       </c>
@@ -3002,7 +2985,7 @@
       <c r="J26" s="1"/>
       <c r="K26" s="6"/>
     </row>
-    <row r="27" spans="1:22">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <v>26</v>
       </c>
@@ -3033,7 +3016,7 @@
       <c r="J27" s="1"/>
       <c r="K27" s="6"/>
     </row>
-    <row r="28" spans="1:22">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>27</v>
       </c>
@@ -3064,7 +3047,7 @@
       <c r="J28" s="1"/>
       <c r="K28" s="6"/>
     </row>
-    <row r="29" spans="1:22">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <v>28</v>
       </c>
@@ -3095,7 +3078,7 @@
       <c r="J29" s="1"/>
       <c r="K29" s="6"/>
     </row>
-    <row r="30" spans="1:22">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <v>29</v>
       </c>
@@ -3126,7 +3109,7 @@
       <c r="J30" s="1"/>
       <c r="K30" s="6"/>
     </row>
-    <row r="31" spans="1:22">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
         <v>30</v>
       </c>
@@ -3157,7 +3140,7 @@
       <c r="J31" s="1"/>
       <c r="K31" s="6"/>
     </row>
-    <row r="32" spans="1:22">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
         <v>31</v>
       </c>
@@ -3188,7 +3171,7 @@
       <c r="J32" s="1"/>
       <c r="K32" s="6"/>
     </row>
-    <row r="33" spans="1:11">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
         <v>32</v>
       </c>
@@ -3219,7 +3202,7 @@
       <c r="J33" s="1"/>
       <c r="K33" s="6"/>
     </row>
-    <row r="34" spans="1:11">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
         <v>33</v>
       </c>
@@ -3250,7 +3233,7 @@
       <c r="J34" s="1"/>
       <c r="K34" s="6"/>
     </row>
-    <row r="35" spans="1:11">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
         <v>34</v>
       </c>
@@ -3281,7 +3264,7 @@
       <c r="J35" s="1"/>
       <c r="K35" s="6"/>
     </row>
-    <row r="36" spans="1:11">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
         <v>35</v>
       </c>
@@ -3312,7 +3295,7 @@
       <c r="J36" s="1"/>
       <c r="K36" s="6"/>
     </row>
-    <row r="37" spans="1:11">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="5"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -3325,7 +3308,7 @@
       <c r="J37" s="1"/>
       <c r="K37" s="6"/>
     </row>
-    <row r="38" spans="1:11">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="5"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -3338,7 +3321,7 @@
       <c r="J38" s="1"/>
       <c r="K38" s="6"/>
     </row>
-    <row r="39" spans="1:11">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="5"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -3351,7 +3334,7 @@
       <c r="J39" s="1"/>
       <c r="K39" s="6"/>
     </row>
-    <row r="40" spans="1:11">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="5"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -3364,7 +3347,7 @@
       <c r="J40" s="1"/>
       <c r="K40" s="6"/>
     </row>
-    <row r="41" spans="1:11">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="5"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -3377,7 +3360,7 @@
       <c r="J41" s="1"/>
       <c r="K41" s="6"/>
     </row>
-    <row r="42" spans="1:11">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="5"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -3390,7 +3373,7 @@
       <c r="J42" s="1"/>
       <c r="K42" s="6"/>
     </row>
-    <row r="43" spans="1:11">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="5"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -3403,7 +3386,7 @@
       <c r="J43" s="1"/>
       <c r="K43" s="6"/>
     </row>
-    <row r="44" spans="1:11">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="5"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -3416,7 +3399,7 @@
       <c r="J44" s="1"/>
       <c r="K44" s="6"/>
     </row>
-    <row r="45" spans="1:11">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="7"/>
       <c r="B45" s="8"/>
       <c r="C45" s="8"/>
@@ -3449,9 +3432,9 @@
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="24">
+    <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
         <v>47</v>
@@ -3478,7 +3461,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -3503,7 +3486,7 @@
       <c r="H2" s="1"/>
       <c r="I2" s="6"/>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -3528,7 +3511,7 @@
       <c r="H3" s="1"/>
       <c r="I3" s="6"/>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -3553,7 +3536,7 @@
       <c r="H4" s="1"/>
       <c r="I4" s="6"/>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -3578,7 +3561,7 @@
       <c r="H5" s="1"/>
       <c r="I5" s="6"/>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -3603,7 +3586,7 @@
       <c r="H6" s="1"/>
       <c r="I6" s="6"/>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -3628,7 +3611,7 @@
       <c r="H7" s="1"/>
       <c r="I7" s="6"/>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -3653,7 +3636,7 @@
       <c r="H8" s="1"/>
       <c r="I8" s="6"/>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -3678,7 +3661,7 @@
       <c r="H9" s="1"/>
       <c r="I9" s="6"/>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -3703,7 +3686,7 @@
       <c r="H10" s="1"/>
       <c r="I10" s="6"/>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -3728,7 +3711,7 @@
       <c r="H11" s="1"/>
       <c r="I11" s="6"/>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
         <v>11</v>
       </c>
@@ -3753,15 +3736,15 @@
       <c r="H12" s="1"/>
       <c r="I12" s="6"/>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H13" s="1"/>
       <c r="I13" s="6"/>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H14" s="1"/>
       <c r="I14" s="6"/>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H15" s="8"/>
       <c r="I15" s="9"/>
     </row>
@@ -3779,9 +3762,9 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="24">
+    <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
         <v>47</v>
@@ -3808,7 +3791,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -3833,7 +3816,7 @@
       <c r="H2" s="1"/>
       <c r="I2" s="6"/>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -3858,7 +3841,7 @@
       <c r="H3" s="1"/>
       <c r="I3" s="6"/>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -3883,7 +3866,7 @@
       <c r="H4" s="1"/>
       <c r="I4" s="6"/>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -3908,7 +3891,7 @@
       <c r="H5" s="1"/>
       <c r="I5" s="6"/>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -3933,7 +3916,7 @@
       <c r="H6" s="1"/>
       <c r="I6" s="6"/>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -3958,7 +3941,7 @@
       <c r="H7" s="1"/>
       <c r="I7" s="6"/>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -3983,7 +3966,7 @@
       <c r="H8" s="1"/>
       <c r="I8" s="6"/>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -4008,7 +3991,7 @@
       <c r="H9" s="1"/>
       <c r="I9" s="6"/>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -4033,7 +4016,7 @@
       <c r="H10" s="1"/>
       <c r="I10" s="6"/>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>10</v>
       </c>
@@ -4058,10 +4041,10 @@
       <c r="H11" s="8"/>
       <c r="I11" s="9"/>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B12" s="8"/>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -4072,7 +4055,7 @@
       <c r="H14" s="3"/>
       <c r="I14" s="4"/>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -4083,7 +4066,7 @@
       <c r="H15" s="1"/>
       <c r="I15" s="6"/>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -4094,7 +4077,7 @@
       <c r="H16" s="1"/>
       <c r="I16" s="6"/>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -4105,7 +4088,7 @@
       <c r="H17" s="1"/>
       <c r="I17" s="6"/>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -4116,7 +4099,7 @@
       <c r="H18" s="1"/>
       <c r="I18" s="6"/>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -4127,7 +4110,7 @@
       <c r="H19" s="1"/>
       <c r="I19" s="6"/>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -4138,7 +4121,7 @@
       <c r="H20" s="1"/>
       <c r="I20" s="6"/>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -4149,7 +4132,7 @@
       <c r="H21" s="1"/>
       <c r="I21" s="6"/>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -4160,7 +4143,7 @@
       <c r="H22" s="1"/>
       <c r="I22" s="6"/>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -4171,7 +4154,7 @@
       <c r="H23" s="1"/>
       <c r="I23" s="6"/>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -4182,7 +4165,7 @@
       <c r="H24" s="1"/>
       <c r="I24" s="6"/>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="7"/>
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
@@ -4206,9 +4189,9 @@
       <selection sqref="A1:K3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" ht="24">
+    <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
         <v>57</v>
@@ -4241,7 +4224,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -4272,7 +4255,7 @@
       <c r="J2" s="1"/>
       <c r="K2" s="6"/>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <v>2</v>
       </c>
@@ -4310,18 +4293,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4542,6 +4525,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9421959D-9476-4FEC-BDFE-1367083D3EBE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44668820-0664-4E62-A660-376AF03334EF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="b60d6f15-5eb1-4c0b-bb71-d899d3bf026f"/>
@@ -4554,14 +4545,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9421959D-9476-4FEC-BDFE-1367083D3EBE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>